<commit_message>
temp and hum added to sis
</commit_message>
<xml_diff>
--- a/GroupElementList.xlsx
+++ b/GroupElementList.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_WEIGHT_SCALE2_NG</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
@@ -1044,19 +1044,29 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" s="1" t="n"/>
+      <c r="B20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>1.816</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
           <t>S_WEIGHT_SCALE2_NG</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>1.815</v>
+        <v>1.816</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1067,107 +1077,97 @@
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>1.816</t>
+          <t>1.830</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Weight scale</t>
+          <t>H2O2 LC sensor</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G21" t="n">
-        <v>1.816</v>
+        <v>1.83</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['M', 'P', 'QIA+', 'XA']</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="n"/>
-      <c r="D22" s="1" t="n"/>
+      <c r="B22" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>1.150</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust air fan</t>
+        </is>
+      </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
+          <t>S_DRIVE</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>1.816</v>
+        <v>1.15</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="inlineStr">
-        <is>
-          <t>1.830</t>
-        </is>
-      </c>
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>H2O2 LC sensor</t>
-        </is>
-      </c>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_SWITCH</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>1.83</v>
+        <v>1.15</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>['M', 'P', 'QIA+', 'XA']</t>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>1.150</t>
-        </is>
-      </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Exhaust air fan</t>
-        </is>
-      </c>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>S_DRIVE</t>
+          <t>S_REG_CONT</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
@@ -1184,56 +1184,76 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
+      <c r="B25" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>1.865</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>S_MOTOR1</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>1.15</v>
+        <v>1.865</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['PSA-', 'V']</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="1" t="n"/>
+      <c r="B26" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>1.866</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>S_REG_CONT</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>1.15</v>
+        <v>1.866</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['PSA-', 'V']</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>1.865</t>
+          <t>1.867</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
@@ -1247,10 +1267,10 @@
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" t="n">
-        <v>1.865</v>
+        <v>1.867</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1261,11 +1281,11 @@
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>1.866</t>
+          <t>1.868</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
@@ -1279,10 +1299,10 @@
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G28" t="n">
-        <v>1.866</v>
+        <v>1.868</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1293,11 +1313,11 @@
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>1.867</t>
+          <t>1.869</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
@@ -1311,10 +1331,10 @@
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G29" t="n">
-        <v>1.867</v>
+        <v>1.869</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1325,11 +1345,11 @@
     <row r="30">
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>1.870</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
@@ -1343,10 +1363,10 @@
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G30" t="n">
-        <v>1.868</v>
+        <v>1.87</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1355,149 +1375,149 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n"/>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_ON_OFF</t>
+        </is>
+      </c>
       <c r="B31" s="1" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>1.869</t>
+          <t>1.690</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Dryer / Humidifier</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G31" t="n">
-        <v>1.869</v>
+        <v>1.69</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['T', 'XA']</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="n">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>1.870</t>
+          <t>1.860</t>
         </is>
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Control valves including 3-way valve</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G32" t="n">
-        <v>1.87</v>
+        <v>1.86</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['V']</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_ON_OFF</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="B33" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>1.705</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>Flow Switch H2O2</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="inlineStr">
-        <is>
-          <t>1.690</t>
-        </is>
-      </c>
-      <c r="D33" s="1" t="inlineStr">
-        <is>
-          <t>Dryer / Humidifier</t>
-        </is>
-      </c>
-      <c r="E33" s="1" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>16</v>
-      </c>
       <c r="G33" t="n">
-        <v>1.69</v>
+        <v>1.705</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>['T', 'XA']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>1.860</t>
+          <t>1.715</t>
         </is>
       </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Control valves including 3-way valve</t>
+          <t>Flow Switch H2O2</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_HI_LO</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1.86</v>
+        <v>1.715</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>['V']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>S_LIMIT_SWITCH</t>
-        </is>
-      </c>
+      <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>1.705</t>
+          <t>1.725</t>
         </is>
       </c>
       <c r="D35" s="1" t="inlineStr">
@@ -1514,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1.705</v>
+        <v>1.725</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1525,75 +1545,75 @@
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.833</t>
         </is>
       </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Flow Switch H2O2</t>
+          <t>TLV H2O2 LC Sensor</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="F36" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G36" t="n">
-        <v>1.715</v>
+        <v>1.833</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
+          <t>['QSA+']</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>1.725</t>
+          <t>1.833</t>
         </is>
       </c>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Flow Switch H2O2</t>
+          <t>TLV H2O2 LC Sensor</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="F37" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>1.725</v>
+        <v>1.833</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
+          <t>['QSA+']</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.834</t>
         </is>
       </c>
       <c r="D38" s="1" t="inlineStr">
@@ -1607,10 +1627,10 @@
         </is>
       </c>
       <c r="F38" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G38" t="n">
-        <v>1.833</v>
+        <v>1.834</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1621,11 +1641,11 @@
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.834</t>
         </is>
       </c>
       <c r="D39" s="1" t="inlineStr">
@@ -1639,10 +1659,10 @@
         </is>
       </c>
       <c r="F39" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G39" t="n">
-        <v>1.833</v>
+        <v>1.834</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1653,75 +1673,75 @@
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>1.834</t>
+          <t>1.901</t>
         </is>
       </c>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>TLV H2O2 LC Sensor</t>
+          <t>Safety door</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_SWITCH</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="F40" s="1" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>1.834</v>
+        <v>1.901</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>['QSA+']</t>
+          <t>['GZA-']</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C41" s="1" t="inlineStr">
         <is>
-          <t>1.834</t>
+          <t>1.902</t>
         </is>
       </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>TLV H2O2 LC Sensor</t>
+          <t>Safety door</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_SWITCH</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="F41" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>1.834</v>
+        <v>1.902</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>['QSA+']</t>
+          <t>['GZA-']</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C42" s="1" t="inlineStr">
         <is>
-          <t>1.901</t>
+          <t>1.903</t>
         </is>
       </c>
       <c r="D42" s="1" t="inlineStr">
@@ -1738,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="G42" t="n">
-        <v>1.901</v>
+        <v>1.903</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1749,11 +1769,11 @@
     <row r="43">
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C43" s="1" t="inlineStr">
         <is>
-          <t>1.902</t>
+          <t>1.904</t>
         </is>
       </c>
       <c r="D43" s="1" t="inlineStr">
@@ -1770,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>1.902</v>
+        <v>1.904</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1781,11 +1801,11 @@
     <row r="44">
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C44" s="1" t="inlineStr">
         <is>
-          <t>1.903</t>
+          <t>1.905</t>
         </is>
       </c>
       <c r="D44" s="1" t="inlineStr">
@@ -1802,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>1.903</v>
+        <v>1.905</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -1813,11 +1833,11 @@
     <row r="45">
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="inlineStr">
         <is>
-          <t>1.904</t>
+          <t>1.906</t>
         </is>
       </c>
       <c r="D45" s="1" t="inlineStr">
@@ -1834,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>1.904</v>
+        <v>1.906</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -1845,16 +1865,16 @@
     <row r="46">
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C46" s="1" t="inlineStr">
         <is>
-          <t>1.905</t>
+          <t>1.911</t>
         </is>
       </c>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Safety door</t>
+          <t>Service cover</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr">
@@ -1863,30 +1883,30 @@
         </is>
       </c>
       <c r="F46" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" t="n">
-        <v>1.905</v>
+        <v>1.911</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>['GZA-']</t>
+          <t>['GSA-']</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C47" s="1" t="inlineStr">
         <is>
-          <t>1.906</t>
+          <t>1.912</t>
         </is>
       </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Safety door</t>
+          <t>Service cover</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr">
@@ -1895,25 +1915,25 @@
         </is>
       </c>
       <c r="F47" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>1.906</v>
+        <v>1.912</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>['GZA-']</t>
+          <t>['GSA-']</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C48" s="1" t="inlineStr">
         <is>
-          <t>1.911</t>
+          <t>1.913</t>
         </is>
       </c>
       <c r="D48" s="1" t="inlineStr">
@@ -1930,7 +1950,7 @@
         <v>2</v>
       </c>
       <c r="G48" t="n">
-        <v>1.911</v>
+        <v>1.913</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -1941,11 +1961,11 @@
     <row r="49">
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C49" s="1" t="inlineStr">
         <is>
-          <t>1.912</t>
+          <t>1.914</t>
         </is>
       </c>
       <c r="D49" s="1" t="inlineStr">
@@ -1962,7 +1982,7 @@
         <v>2</v>
       </c>
       <c r="G49" t="n">
-        <v>1.912</v>
+        <v>1.914</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -1973,11 +1993,11 @@
     <row r="50">
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C50" s="1" t="inlineStr">
         <is>
-          <t>1.913</t>
+          <t>1.915</t>
         </is>
       </c>
       <c r="D50" s="1" t="inlineStr">
@@ -1991,10 +2011,10 @@
         </is>
       </c>
       <c r="F50" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G50" t="n">
-        <v>1.913</v>
+        <v>1.915</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2005,11 +2025,11 @@
     <row r="51">
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="inlineStr">
         <is>
-          <t>1.914</t>
+          <t>1.916</t>
         </is>
       </c>
       <c r="D51" s="1" t="inlineStr">
@@ -2023,10 +2043,10 @@
         </is>
       </c>
       <c r="F51" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G51" t="n">
-        <v>1.914</v>
+        <v>1.916</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2037,11 +2057,11 @@
     <row r="52">
       <c r="A52" s="1" t="n"/>
       <c r="B52" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C52" s="1" t="inlineStr">
         <is>
-          <t>1.915</t>
+          <t>1.917</t>
         </is>
       </c>
       <c r="D52" s="1" t="inlineStr">
@@ -2058,7 +2078,7 @@
         <v>3</v>
       </c>
       <c r="G52" t="n">
-        <v>1.915</v>
+        <v>1.917</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2069,11 +2089,11 @@
     <row r="53">
       <c r="A53" s="1" t="n"/>
       <c r="B53" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C53" s="1" t="inlineStr">
         <is>
-          <t>1.916</t>
+          <t>1.918</t>
         </is>
       </c>
       <c r="D53" s="1" t="inlineStr">
@@ -2090,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="G53" t="n">
-        <v>1.916</v>
+        <v>1.918</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2101,11 +2121,11 @@
     <row r="54">
       <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C54" s="1" t="inlineStr">
         <is>
-          <t>1.917</t>
+          <t>1.919</t>
         </is>
       </c>
       <c r="D54" s="1" t="inlineStr">
@@ -2122,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="G54" t="n">
-        <v>1.917</v>
+        <v>1.919</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2133,16 +2153,16 @@
     <row r="55">
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C55" s="1" t="inlineStr">
         <is>
-          <t>1.918</t>
+          <t>1.921</t>
         </is>
       </c>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Service cover</t>
+          <t>Mousehole door</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr">
@@ -2151,30 +2171,30 @@
         </is>
       </c>
       <c r="F55" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G55" t="n">
-        <v>1.918</v>
+        <v>1.921</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>['GSA-']</t>
+          <t>['GZA-']</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C56" s="1" t="inlineStr">
         <is>
-          <t>1.919</t>
+          <t>1.922</t>
         </is>
       </c>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Service cover</t>
+          <t>Mousehole door</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr">
@@ -2183,25 +2203,25 @@
         </is>
       </c>
       <c r="F56" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G56" t="n">
-        <v>1.919</v>
+        <v>1.922</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>['GSA-']</t>
+          <t>['GZA-']</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
       <c r="B57" s="1" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1" t="inlineStr">
         <is>
-          <t>1.921</t>
+          <t>1.923</t>
         </is>
       </c>
       <c r="D57" s="1" t="inlineStr">
@@ -2215,10 +2235,10 @@
         </is>
       </c>
       <c r="F57" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G57" t="n">
-        <v>1.921</v>
+        <v>1.923</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2229,11 +2249,11 @@
     <row r="58">
       <c r="A58" s="1" t="n"/>
       <c r="B58" s="1" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C58" s="1" t="inlineStr">
         <is>
-          <t>1.922</t>
+          <t>1.924</t>
         </is>
       </c>
       <c r="D58" s="1" t="inlineStr">
@@ -2247,10 +2267,10 @@
         </is>
       </c>
       <c r="F58" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G58" t="n">
-        <v>1.922</v>
+        <v>1.924</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -2261,75 +2281,75 @@
     <row r="59">
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="n">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="inlineStr">
         <is>
-          <t>1.923</t>
+          <t>2.705</t>
         </is>
       </c>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Mousehole door</t>
+          <t>Flow Switch H2O2</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F59" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G59" t="n">
-        <v>1.923</v>
+        <v>2.705</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>['GZA-']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C60" s="1" t="inlineStr">
         <is>
-          <t>1.924</t>
+          <t>2.715</t>
         </is>
       </c>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>Mousehole door</t>
+          <t>Flow Switch H2O2</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F60" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G60" t="n">
-        <v>1.924</v>
+        <v>2.715</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>['GZA-']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
       <c r="B61" s="1" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C61" s="1" t="inlineStr">
         <is>
-          <t>2.705</t>
+          <t>2.725</t>
         </is>
       </c>
       <c r="D61" s="1" t="inlineStr">
@@ -2346,7 +2366,7 @@
         <v>2</v>
       </c>
       <c r="G61" t="n">
-        <v>2.705</v>
+        <v>2.725</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -2355,91 +2375,71 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
       <c r="B62" s="1" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t>2.715</t>
+          <t>1.150</t>
         </is>
       </c>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>Flow Switch H2O2</t>
+          <t>Exhaust air fan</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_DRIVE</t>
         </is>
       </c>
       <c r="F62" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G62" t="n">
-        <v>2.715</v>
+        <v>1.15</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="C63" s="1" t="inlineStr">
-        <is>
-          <t>2.725</t>
-        </is>
-      </c>
-      <c r="D63" s="1" t="inlineStr">
-        <is>
-          <t>Flow Switch H2O2</t>
-        </is>
-      </c>
+      <c r="B63" s="1" t="n"/>
+      <c r="C63" s="1" t="n"/>
+      <c r="D63" s="1" t="n"/>
       <c r="E63" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F63" s="1" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G63" t="n">
-        <v>2.725</v>
+        <v>1.15</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>S_MOTOR1</t>
-        </is>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C64" s="1" t="inlineStr">
-        <is>
-          <t>1.150</t>
-        </is>
-      </c>
-      <c r="D64" s="1" t="inlineStr">
-        <is>
-          <t>Exhaust air fan</t>
-        </is>
-      </c>
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="n"/>
+      <c r="D64" s="1" t="n"/>
       <c r="E64" s="1" t="inlineStr">
         <is>
-          <t>S_DRIVE</t>
+          <t>S_REG_CONT</t>
         </is>
       </c>
       <c r="F64" s="1" t="n">
@@ -2456,56 +2456,76 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="n"/>
-      <c r="C65" s="1" t="n"/>
-      <c r="D65" s="1" t="n"/>
+      <c r="B65" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>1.550</t>
+        </is>
+      </c>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust air flap</t>
+        </is>
+      </c>
       <c r="E65" s="1" t="inlineStr">
         <is>
           <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F65" s="1" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G65" t="n">
-        <v>1.15</v>
+        <v>1.55</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
-      <c r="D66" s="1" t="n"/>
+      <c r="B66" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>1.555</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust bypass valve</t>
+        </is>
+      </c>
       <c r="E66" s="1" t="inlineStr">
         <is>
-          <t>S_REG_CONT</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F66" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G66" t="n">
-        <v>1.15</v>
+        <v>1.555</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['GIA', 'V', 'Y', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
       <c r="B67" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C67" s="1" t="inlineStr">
         <is>
-          <t>1.550</t>
+          <t>1.560</t>
         </is>
       </c>
       <c r="D67" s="1" t="inlineStr">
@@ -2519,10 +2539,10 @@
         </is>
       </c>
       <c r="F67" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G67" t="n">
-        <v>1.55</v>
+        <v>1.56</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -2533,16 +2553,16 @@
     <row r="68">
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1" t="inlineStr">
         <is>
-          <t>1.555</t>
+          <t>1.655</t>
         </is>
       </c>
       <c r="D68" s="1" t="inlineStr">
         <is>
-          <t>Exhaust bypass valve</t>
+          <t>Control valve</t>
         </is>
       </c>
       <c r="E68" s="1" t="inlineStr">
@@ -2551,62 +2571,52 @@
         </is>
       </c>
       <c r="F68" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G68" t="n">
-        <v>1.555</v>
+        <v>1.655</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>['GIA', 'V', 'Y', 'YC']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C69" s="1" t="inlineStr">
-        <is>
-          <t>1.560</t>
-        </is>
-      </c>
-      <c r="D69" s="1" t="inlineStr">
-        <is>
-          <t>Exhaust air flap</t>
-        </is>
-      </c>
+      <c r="B69" s="1" t="n"/>
+      <c r="C69" s="1" t="n"/>
+      <c r="D69" s="1" t="n"/>
       <c r="E69" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_HI_LO</t>
+          <t>S_REG_CONT</t>
         </is>
       </c>
       <c r="F69" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G69" t="n">
-        <v>1.56</v>
+        <v>1.655</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>['GIA', 'K', 'Y', 'YC']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C70" s="1" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>1.680</t>
         </is>
       </c>
       <c r="D70" s="1" t="inlineStr">
         <is>
-          <t>Control valve</t>
+          <t>Electric heating</t>
         </is>
       </c>
       <c r="E70" s="1" t="inlineStr">
@@ -2618,11 +2628,11 @@
         <v>11</v>
       </c>
       <c r="G70" t="n">
-        <v>1.655</v>
+        <v>1.68</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>['H', 'M', 'NC']</t>
+          <t>['EC', 'TSA+']</t>
         </is>
       </c>
     </row>
@@ -2637,115 +2647,121 @@
         </is>
       </c>
       <c r="F71" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G71" t="n">
-        <v>1.655</v>
+        <v>1.68</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>['H', 'M', 'NC']</t>
+          <t>['EC', 'TSA+']</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
       <c r="B72" s="1" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C72" s="1" t="inlineStr">
         <is>
-          <t>1.680</t>
+          <t>1.825</t>
         </is>
       </c>
       <c r="D72" s="1" t="inlineStr">
         <is>
-          <t>Electric heating</t>
+          <t>Flow rate sensor</t>
         </is>
       </c>
       <c r="E72" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_HI_LO</t>
+          <t>S_REG_CONT</t>
         </is>
       </c>
       <c r="F72" s="1" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G72" t="n">
-        <v>1.68</v>
+        <v>1.825</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>['EC', 'TSA+']</t>
+          <t>['FIA+', 'H', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="n"/>
-      <c r="C73" s="1" t="n"/>
-      <c r="D73" s="1" t="n"/>
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>1.700</t>
+        </is>
+      </c>
+      <c r="D73" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
       <c r="E73" s="1" t="inlineStr">
         <is>
-          <t>S_REG_CONT</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F73" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G73" t="n">
-        <v>1.68</v>
+        <v>1.7</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>['EC', 'TSA+']</t>
+          <t>['M', 'P', 'SC']</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="n">
-        <v>15</v>
-      </c>
+      <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="inlineStr">
         <is>
-          <t>1.825</t>
+          <t>1.710</t>
         </is>
       </c>
       <c r="D74" s="1" t="inlineStr">
         <is>
-          <t>Flow rate sensor</t>
+          <t>Peristaltic pump</t>
         </is>
       </c>
       <c r="E74" s="1" t="inlineStr">
         <is>
-          <t>S_REG_CONT</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F74" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G74" t="n">
-        <v>1.825</v>
+        <v>1.71</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>['FIA+', 'H', 'YC']</t>
+          <t>['M', 'P', 'SC']</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>S_PUMP_TEST</t>
-        </is>
-      </c>
-      <c r="B75" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A75" s="1" t="n"/>
+      <c r="B75" s="1" t="n"/>
       <c r="C75" s="1" t="inlineStr">
         <is>
-          <t>1.700</t>
+          <t>1.720</t>
         </is>
       </c>
       <c r="D75" s="1" t="inlineStr">
@@ -2762,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>1.7</v>
+        <v>1.72</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
@@ -2772,10 +2788,12 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n"/>
+      <c r="B76" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C76" s="1" t="inlineStr">
         <is>
-          <t>1.710</t>
+          <t>2.700</t>
         </is>
       </c>
       <c r="D76" s="1" t="inlineStr">
@@ -2789,10 +2807,10 @@
         </is>
       </c>
       <c r="F76" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G76" t="n">
-        <v>1.71</v>
+        <v>2.7</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -2805,7 +2823,7 @@
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="inlineStr">
         <is>
-          <t>1.720</t>
+          <t>2.710</t>
         </is>
       </c>
       <c r="D77" s="1" t="inlineStr">
@@ -2819,10 +2837,10 @@
         </is>
       </c>
       <c r="F77" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
-        <v>1.72</v>
+        <v>2.71</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -2832,12 +2850,10 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="B78" s="1" t="n"/>
       <c r="C78" s="1" t="inlineStr">
         <is>
-          <t>2.700</t>
+          <t>2.720</t>
         </is>
       </c>
       <c r="D78" s="1" t="inlineStr">
@@ -2854,7 +2870,7 @@
         <v>2</v>
       </c>
       <c r="G78" t="n">
-        <v>2.7</v>
+        <v>2.72</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -2863,91 +2879,75 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="n"/>
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>S_REG_CONT</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C79" s="1" t="inlineStr">
         <is>
-          <t>2.710</t>
+          <t>1.150</t>
         </is>
       </c>
       <c r="D79" s="1" t="inlineStr">
         <is>
-          <t>Peristaltic pump</t>
+          <t>Exhaust air fan</t>
         </is>
       </c>
       <c r="E79" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_DRIVE</t>
         </is>
       </c>
       <c r="F79" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G79" t="n">
-        <v>2.71</v>
+        <v>1.15</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['M', 'P', 'SC']</t>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
       <c r="B80" s="1" t="n"/>
-      <c r="C80" s="1" t="inlineStr">
-        <is>
-          <t>2.720</t>
-        </is>
-      </c>
-      <c r="D80" s="1" t="inlineStr">
-        <is>
-          <t>Peristaltic pump</t>
-        </is>
-      </c>
+      <c r="C80" s="1" t="n"/>
+      <c r="D80" s="1" t="n"/>
       <c r="E80" s="1" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F80" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>['M', 'SC', 'TSA+', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n"/>
+      <c r="B81" s="1" t="n"/>
+      <c r="C81" s="1" t="n"/>
+      <c r="D81" s="1" t="n"/>
+      <c r="E81" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
+      <c r="F81" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="G80" t="n">
-        <v>2.72</v>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>['M', 'P', 'SC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>S_REG_CONT</t>
-        </is>
-      </c>
-      <c r="B81" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C81" s="1" t="inlineStr">
-        <is>
-          <t>1.150</t>
-        </is>
-      </c>
-      <c r="D81" s="1" t="inlineStr">
-        <is>
-          <t>Exhaust air fan</t>
-        </is>
-      </c>
-      <c r="E81" s="1" t="inlineStr">
-        <is>
-          <t>S_DRIVE</t>
-        </is>
-      </c>
-      <c r="F81" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="G81" t="n">
         <v>1.15</v>
@@ -2960,23 +2960,33 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="n"/>
-      <c r="C82" s="1" t="n"/>
-      <c r="D82" s="1" t="n"/>
+      <c r="B82" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>1.655</t>
+        </is>
+      </c>
+      <c r="D82" s="1" t="inlineStr">
+        <is>
+          <t>Control valve</t>
+        </is>
+      </c>
       <c r="E82" s="1" t="inlineStr">
         <is>
           <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F82" s="1" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G82" t="n">
-        <v>1.15</v>
+        <v>1.655</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
@@ -2991,30 +3001,30 @@
         </is>
       </c>
       <c r="F83" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G83" t="n">
-        <v>1.15</v>
+        <v>1.655</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>['M', 'SC', 'TSA+', 'V']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
       <c r="B84" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84" s="1" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>1.680</t>
         </is>
       </c>
       <c r="D84" s="1" t="inlineStr">
         <is>
-          <t>Control valve</t>
+          <t>Electric heating</t>
         </is>
       </c>
       <c r="E84" s="1" t="inlineStr">
@@ -3026,11 +3036,11 @@
         <v>11</v>
       </c>
       <c r="G84" t="n">
-        <v>1.655</v>
+        <v>1.68</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>['H', 'M', 'NC']</t>
+          <t>['EC', 'TSA+']</t>
         </is>
       </c>
     </row>
@@ -3045,83 +3055,89 @@
         </is>
       </c>
       <c r="F85" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G85" t="n">
-        <v>1.655</v>
+        <v>1.68</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>['H', 'M', 'NC']</t>
+          <t>['EC', 'TSA+']</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n"/>
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
       <c r="B86" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" s="1" t="inlineStr">
         <is>
-          <t>1.680</t>
+          <t>1.700</t>
         </is>
       </c>
       <c r="D86" s="1" t="inlineStr">
         <is>
-          <t>Electric heating</t>
+          <t>Peristaltic pump</t>
         </is>
       </c>
       <c r="E86" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_HI_LO</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="F86" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G86" t="n">
-        <v>1.68</v>
+        <v>1.7</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>['EC', 'TSA+']</t>
+          <t>['M', 'P', 'SC']</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
       <c r="B87" s="1" t="n"/>
-      <c r="C87" s="1" t="n"/>
-      <c r="D87" s="1" t="n"/>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>1.705</t>
+        </is>
+      </c>
+      <c r="D87" s="1" t="inlineStr">
+        <is>
+          <t>Flow Switch H2O2</t>
+        </is>
+      </c>
       <c r="E87" s="1" t="inlineStr">
         <is>
-          <t>S_MOTOR1</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="F87" s="1" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G87" t="n">
-        <v>1.68</v>
+        <v>1.705</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>['EC', 'TSA+']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>S_SIS</t>
-        </is>
-      </c>
-      <c r="B88" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A88" s="1" t="n"/>
+      <c r="B88" s="1" t="n"/>
       <c r="C88" s="1" t="inlineStr">
         <is>
-          <t>1.700</t>
+          <t>1.710</t>
         </is>
       </c>
       <c r="D88" s="1" t="inlineStr">
@@ -3138,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="G88" t="n">
-        <v>1.7</v>
+        <v>1.71</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -3151,7 +3167,7 @@
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="inlineStr">
         <is>
-          <t>1.705</t>
+          <t>1.715</t>
         </is>
       </c>
       <c r="D89" s="1" t="inlineStr">
@@ -3165,10 +3181,10 @@
         </is>
       </c>
       <c r="F89" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G89" t="n">
-        <v>1.705</v>
+        <v>1.715</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
@@ -3181,7 +3197,7 @@
       <c r="B90" s="1" t="n"/>
       <c r="C90" s="1" t="inlineStr">
         <is>
-          <t>1.710</t>
+          <t>1.720</t>
         </is>
       </c>
       <c r="D90" s="1" t="inlineStr">
@@ -3198,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>1.71</v>
+        <v>1.72</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
@@ -3211,7 +3227,7 @@
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="1" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.725</t>
         </is>
       </c>
       <c r="D91" s="1" t="inlineStr">
@@ -3225,10 +3241,10 @@
         </is>
       </c>
       <c r="F91" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G91" t="n">
-        <v>1.715</v>
+        <v>1.725</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
@@ -3241,28 +3257,28 @@
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="inlineStr">
         <is>
-          <t>1.720</t>
+          <t>1.800</t>
         </is>
       </c>
       <c r="D92" s="1" t="inlineStr">
         <is>
-          <t>Peristaltic pump</t>
+          <t>Temperature sensor</t>
         </is>
       </c>
       <c r="E92" s="1" t="inlineStr">
         <is>
-          <t>S_PUMP_TEST</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F92" s="1" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G92" t="n">
-        <v>1.72</v>
+        <v>1.8</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>['M', 'P', 'SC']</t>
+          <t>['TICA±']</t>
         </is>
       </c>
     </row>
@@ -3271,42 +3287,44 @@
       <c r="B93" s="1" t="n"/>
       <c r="C93" s="1" t="inlineStr">
         <is>
-          <t>1.725</t>
+          <t>1.810</t>
         </is>
       </c>
       <c r="D93" s="1" t="inlineStr">
         <is>
-          <t>Flow Switch H2O2</t>
+          <t>Humidity sensor</t>
         </is>
       </c>
       <c r="E93" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_SWITCH</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F93" s="1" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G93" t="n">
-        <v>1.725</v>
+        <v>1.81</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
+          <t>['MIA±']</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="n"/>
+      <c r="B94" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C94" s="1" t="inlineStr">
         <is>
-          <t>1.815</t>
+          <t>1.800</t>
         </is>
       </c>
       <c r="D94" s="1" t="inlineStr">
         <is>
-          <t>Weight scale</t>
+          <t>Temperature sensor</t>
         </is>
       </c>
       <c r="E94" s="1" t="inlineStr">
@@ -3315,90 +3333,104 @@
         </is>
       </c>
       <c r="F94" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G94" t="n">
-        <v>1.815</v>
+        <v>1.8</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['TICA±']</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
       <c r="B95" s="1" t="n"/>
-      <c r="C95" s="1" t="n"/>
-      <c r="D95" s="1" t="n"/>
+      <c r="C95" s="1" t="inlineStr">
+        <is>
+          <t>1.810</t>
+        </is>
+      </c>
+      <c r="D95" s="1" t="inlineStr">
+        <is>
+          <t>Humidity sensor</t>
+        </is>
+      </c>
       <c r="E95" s="1" t="inlineStr">
         <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="F95" s="1" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G95" t="n">
-        <v>1.815</v>
+        <v>1.81</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['MIA±']</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="1" t="n"/>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>2.700</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E96" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F96" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C96" s="1" t="inlineStr">
-        <is>
-          <t>1.816</t>
-        </is>
-      </c>
-      <c r="D96" s="1" t="inlineStr">
-        <is>
-          <t>Weight scale</t>
-        </is>
-      </c>
-      <c r="E96" s="1" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="F96" s="1" t="n">
-        <v>18</v>
-      </c>
       <c r="G96" t="n">
-        <v>1.816</v>
+        <v>2.7</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['M', 'P', 'SC']</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
       <c r="B97" s="1" t="n"/>
-      <c r="C97" s="1" t="n"/>
-      <c r="D97" s="1" t="n"/>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>2.705</t>
+        </is>
+      </c>
+      <c r="D97" s="1" t="inlineStr">
+        <is>
+          <t>Flow Switch H2O2</t>
+        </is>
+      </c>
       <c r="E97" s="1" t="inlineStr">
         <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
+          <t>S_LIMIT_SWITCH</t>
         </is>
       </c>
       <c r="F97" s="1" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="G97" t="n">
-        <v>1.816</v>
+        <v>2.705</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>['WICA±']</t>
+          <t>['LSA-']</t>
         </is>
       </c>
     </row>
@@ -3407,7 +3439,7 @@
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="inlineStr">
         <is>
-          <t>2.700</t>
+          <t>2.710</t>
         </is>
       </c>
       <c r="D98" s="1" t="inlineStr">
@@ -3424,7 +3456,7 @@
         <v>2</v>
       </c>
       <c r="G98" t="n">
-        <v>2.7</v>
+        <v>2.71</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
@@ -3437,7 +3469,7 @@
       <c r="B99" s="1" t="n"/>
       <c r="C99" s="1" t="inlineStr">
         <is>
-          <t>2.705</t>
+          <t>2.715</t>
         </is>
       </c>
       <c r="D99" s="1" t="inlineStr">
@@ -3451,10 +3483,10 @@
         </is>
       </c>
       <c r="F99" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G99" t="n">
-        <v>2.705</v>
+        <v>2.715</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -3467,7 +3499,7 @@
       <c r="B100" s="1" t="n"/>
       <c r="C100" s="1" t="inlineStr">
         <is>
-          <t>2.710</t>
+          <t>2.720</t>
         </is>
       </c>
       <c r="D100" s="1" t="inlineStr">
@@ -3484,7 +3516,7 @@
         <v>2</v>
       </c>
       <c r="G100" t="n">
-        <v>2.71</v>
+        <v>2.72</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -3497,7 +3529,7 @@
       <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="inlineStr">
         <is>
-          <t>2.715</t>
+          <t>2.725</t>
         </is>
       </c>
       <c r="D101" s="1" t="inlineStr">
@@ -3511,10 +3543,10 @@
         </is>
       </c>
       <c r="F101" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G101" t="n">
-        <v>2.715</v>
+        <v>2.725</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
@@ -3523,238 +3555,118 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n"/>
-      <c r="B102" s="1" t="n"/>
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="B102" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C102" s="1" t="inlineStr">
         <is>
-          <t>2.720</t>
+          <t>1.815</t>
         </is>
       </c>
       <c r="D102" s="1" t="inlineStr">
         <is>
-          <t>Peristaltic pump</t>
+          <t>Weight scale</t>
         </is>
       </c>
       <c r="E102" s="1" t="inlineStr">
         <is>
-          <t>S_PUMP_TEST</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F102" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G102" t="n">
-        <v>2.72</v>
+        <v>1.815</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>['M', 'P', 'SC']</t>
+          <t>['WICA±']</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
-      <c r="B103" s="1" t="n"/>
+      <c r="B103" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C103" s="1" t="inlineStr">
         <is>
-          <t>2.725</t>
+          <t>1.816</t>
         </is>
       </c>
       <c r="D103" s="1" t="inlineStr">
         <is>
-          <t>Flow Switch H2O2</t>
+          <t>Weight scale</t>
         </is>
       </c>
       <c r="E103" s="1" t="inlineStr">
         <is>
-          <t>S_LIMIT_SWITCH</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="F103" s="1" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G103" t="n">
-        <v>2.725</v>
+        <v>1.816</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>['LSA-']</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="inlineStr">
-        <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
-        </is>
-      </c>
-      <c r="B104" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1" t="inlineStr">
-        <is>
-          <t>1.815</t>
-        </is>
-      </c>
-      <c r="D104" s="1" t="inlineStr">
-        <is>
-          <t>Weight scale</t>
-        </is>
-      </c>
-      <c r="E104" s="1" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="F104" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="G104" t="n">
-        <v>1.815</v>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
           <t>['WICA±']</t>
         </is>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="1" t="n"/>
-      <c r="B105" s="1" t="n"/>
-      <c r="C105" s="1" t="n"/>
-      <c r="D105" s="1" t="n"/>
-      <c r="E105" s="1" t="inlineStr">
-        <is>
-          <t>S_SIS</t>
-        </is>
-      </c>
-      <c r="F105" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G105" t="n">
-        <v>1.815</v>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>['WICA±']</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n"/>
-      <c r="B106" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C106" s="1" t="inlineStr">
-        <is>
-          <t>1.816</t>
-        </is>
-      </c>
-      <c r="D106" s="1" t="inlineStr">
-        <is>
-          <t>Weight scale</t>
-        </is>
-      </c>
-      <c r="E106" s="1" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="F106" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="G106" t="n">
-        <v>1.816</v>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>['WICA±']</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n"/>
-      <c r="B107" s="1" t="n"/>
-      <c r="C107" s="1" t="n"/>
-      <c r="D107" s="1" t="n"/>
-      <c r="E107" s="1" t="inlineStr">
-        <is>
-          <t>S_SIS</t>
-        </is>
-      </c>
-      <c r="F107" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G107" t="n">
-        <v>1.816</v>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>['WICA±']</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="43">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A63"/>
-    <mergeCell ref="A64:A74"/>
-    <mergeCell ref="A75:A80"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="A88:A103"/>
-    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A11:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A61"/>
+    <mergeCell ref="A62:A72"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A86:A101"/>
+    <mergeCell ref="A102:A103"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B68:B69"/>
     <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="B82:B83"/>
     <mergeCell ref="B84:B85"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="B88:B95"/>
-    <mergeCell ref="B96:B103"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="B86:B93"/>
+    <mergeCell ref="B94:B101"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C68:C69"/>
     <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="C82:C83"/>
     <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="C106:C107"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D68:D69"/>
     <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="D82:D83"/>
     <mergeCell ref="D84:D85"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="D106:D107"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>